<commit_message>
improved way to search semantic tables
</commit_message>
<xml_diff>
--- a/src/utils/data/semantics_data.xlsx
+++ b/src/utils/data/semantics_data.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauth\OneDrive\Desktop\sql_assistant_v3\src\utils\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C94F01-F6AC-4E29-9A37-4638C3AC7043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9298A46-BA3E-4222-A9FA-74A435ABD281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="7992" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{AFE3706E-D2E0-4CCB-B251-2FC4B29F0B89}"/>
+    <workbookView xWindow="22932" yWindow="7992" windowWidth="23256" windowHeight="12456" tabRatio="757" activeTab="1" xr2:uid="{AFE3706E-D2E0-4CCB-B251-2FC4B29F0B89}"/>
   </bookViews>
   <sheets>
     <sheet name="semantics_tables" sheetId="1" r:id="rId1"/>
-    <sheet name="semantics_relations" sheetId="2" r:id="rId2"/>
-    <sheet name="semantics_columns" sheetId="3" r:id="rId3"/>
-    <sheet name="basic_columns" sheetId="4" r:id="rId4"/>
-    <sheet name="relations" sheetId="5" r:id="rId5"/>
+    <sheet name="semantic_tables_kw" sheetId="6" r:id="rId2"/>
+    <sheet name="semantics_relations" sheetId="2" r:id="rId3"/>
+    <sheet name="semantics_relations_kw" sheetId="7" r:id="rId4"/>
+    <sheet name="semantics_columns" sheetId="3" r:id="rId5"/>
+    <sheet name="basic_columns" sheetId="4" r:id="rId6"/>
+    <sheet name="relations" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">basic_columns!$B$1:$F$62</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">semantics_columns!$A$1:$G$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">basic_columns!$B$1:$F$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">semantics_columns!$A$1:$G$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="407">
   <si>
     <t>semantic_table_description</t>
   </si>
@@ -517,9 +519,6 @@
     <t>fluid name</t>
   </si>
   <si>
-    <t>fluid abbreviature</t>
-  </si>
-  <si>
     <t>fluid status</t>
   </si>
   <si>
@@ -535,9 +534,6 @@
     <t>measurement system tag</t>
   </si>
   <si>
-    <t>measurement system interface visibility</t>
-  </si>
-  <si>
     <t>measurement type identificator</t>
   </si>
   <si>
@@ -547,9 +543,6 @@
     <t>measurement type status</t>
   </si>
   <si>
-    <t>measurement system usage</t>
-  </si>
-  <si>
     <t>data type identificator</t>
   </si>
   <si>
@@ -604,84 +597,21 @@
     <t>modbus map tag label</t>
   </si>
   <si>
-    <t>modbus map tag index</t>
-  </si>
-  <si>
-    <t>modbus map OPC tag</t>
-  </si>
-  <si>
-    <t>modbus map register</t>
-  </si>
-  <si>
     <t>modbus map point</t>
   </si>
   <si>
     <t>modbus map logic number</t>
   </si>
   <si>
-    <t>modbus map function</t>
-  </si>
-  <si>
     <t>flow computer identificator</t>
   </si>
   <si>
     <t>flow computer port number</t>
   </si>
   <si>
-    <t>flow computer secondary port number</t>
-  </si>
-  <si>
-    <t>flow computer modicon compatibility</t>
-  </si>
-  <si>
     <t>flow computer status</t>
   </si>
   <si>
-    <t>flow computer real time lecture</t>
-  </si>
-  <si>
-    <t>flow computer configuration lecture</t>
-  </si>
-  <si>
-    <t>flow computer alarma configuration</t>
-  </si>
-  <si>
-    <t>flow computer events configuration</t>
-  </si>
-  <si>
-    <t>flow computer historic lecture</t>
-  </si>
-  <si>
-    <t>flow computer destiny group</t>
-  </si>
-  <si>
-    <t>flow computer desnity unit</t>
-  </si>
-  <si>
-    <t>flow computer source group</t>
-  </si>
-  <si>
-    <t>flow computer source unit</t>
-  </si>
-  <si>
-    <t>flow computer schedule</t>
-  </si>
-  <si>
-    <t>flow computer batch</t>
-  </si>
-  <si>
-    <t>flow computer protocol type</t>
-  </si>
-  <si>
-    <t>flow computer historic process</t>
-  </si>
-  <si>
-    <t>flow computer real time process</t>
-  </si>
-  <si>
-    <t>flow computer OPC server</t>
-  </si>
-  <si>
     <t>flow computer meter system code</t>
   </si>
   <si>
@@ -694,12 +624,6 @@
     <t>variable name</t>
   </si>
   <si>
-    <t>variable report</t>
-  </si>
-  <si>
-    <t>variable chromatography</t>
-  </si>
-  <si>
     <t>variable status</t>
   </si>
   <si>
@@ -718,57 +642,18 @@
     <t>equipment serial</t>
   </si>
   <si>
-    <t>equipment calibration date</t>
-  </si>
-  <si>
-    <t>equipment model</t>
-  </si>
-  <si>
-    <t>equipment features</t>
-  </si>
-  <si>
     <t>equipment status</t>
   </si>
   <si>
-    <t>equipment planification</t>
-  </si>
-  <si>
-    <t>equipment category</t>
-  </si>
-  <si>
     <t>equipment type identificator</t>
   </si>
   <si>
     <t>equipment type name</t>
   </si>
   <si>
-    <t>equipment type aslef configuration</t>
-  </si>
-  <si>
-    <t>equipment type meteorologic status</t>
-  </si>
-  <si>
-    <t>equipment type certified name</t>
-  </si>
-  <si>
-    <t>equipment type report</t>
-  </si>
-  <si>
-    <t>equipment type multivariable option</t>
-  </si>
-  <si>
-    <t>equipment type max equipment number</t>
-  </si>
-  <si>
-    <t>equipment type Termo behavior</t>
-  </si>
-  <si>
     <t>equipment type status</t>
   </si>
   <si>
-    <t>equipment type analysis feature</t>
-  </si>
-  <si>
     <t>manufacturer identificator</t>
   </si>
   <si>
@@ -793,9 +678,6 @@
     <t>measurement system equipment status</t>
   </si>
   <si>
-    <t>measurement system equipment sensors</t>
-  </si>
-  <si>
     <t>flow computer name</t>
   </si>
   <si>
@@ -844,9 +726,6 @@
     <t>SubTipoFluido</t>
   </si>
   <si>
-    <t>measurement system sub fluid type</t>
-  </si>
-  <si>
     <t>Exclusively reffers to subtype natural gas DIF or LIN, use only when fluid type fk id=1</t>
   </si>
   <si>
@@ -1216,16 +1095,178 @@
     <t>Every measurement system is located in Platform/installation.</t>
   </si>
   <si>
-    <t>platform installation abbreviation</t>
-  </si>
-  <si>
-    <t>platform installation interface visibility</t>
-  </si>
-  <si>
     <t>platform installation name</t>
   </si>
   <si>
     <t>TopeMaxEquXSistemasMed</t>
+  </si>
+  <si>
+    <t>equipment type</t>
+  </si>
+  <si>
+    <t>equipments measurement system</t>
+  </si>
+  <si>
+    <t>platform, installation</t>
+  </si>
+  <si>
+    <t>meters, measurement system, flow computer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flow computers </t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>measurement system</t>
+  </si>
+  <si>
+    <t>flow computer</t>
+  </si>
+  <si>
+    <t>fluid</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>firmware</t>
+  </si>
+  <si>
+    <t>measure type</t>
+  </si>
+  <si>
+    <t>flow computer type</t>
+  </si>
+  <si>
+    <t>flow computers types</t>
+  </si>
+  <si>
+    <t>interface visibility</t>
+  </si>
+  <si>
+    <t>abbreviature</t>
+  </si>
+  <si>
+    <t>sub fluid</t>
+  </si>
+  <si>
+    <t>usage</t>
+  </si>
+  <si>
+    <t>tag index</t>
+  </si>
+  <si>
+    <t>OPC tag</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>secondary port</t>
+  </si>
+  <si>
+    <t>modicon compatibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> real time lecture</t>
+  </si>
+  <si>
+    <t>configuration lecture</t>
+  </si>
+  <si>
+    <t>alarm configuration</t>
+  </si>
+  <si>
+    <t>events configuration</t>
+  </si>
+  <si>
+    <t>historic lecture</t>
+  </si>
+  <si>
+    <t>destiny group</t>
+  </si>
+  <si>
+    <t>desnity unit</t>
+  </si>
+  <si>
+    <t>source group</t>
+  </si>
+  <si>
+    <t>source unit</t>
+  </si>
+  <si>
+    <t>schedule</t>
+  </si>
+  <si>
+    <t>fbatch</t>
+  </si>
+  <si>
+    <t>protocol type</t>
+  </si>
+  <si>
+    <t>historic process</t>
+  </si>
+  <si>
+    <t>real time process</t>
+  </si>
+  <si>
+    <t>OPC server</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>chromatography</t>
+  </si>
+  <si>
+    <t>calibration date</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>features</t>
+  </si>
+  <si>
+    <t>planification</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>aslef configuration</t>
+  </si>
+  <si>
+    <t>meteorologic status</t>
+  </si>
+  <si>
+    <t>certified name</t>
+  </si>
+  <si>
+    <t>multivariable option</t>
+  </si>
+  <si>
+    <t>max equipment number</t>
+  </si>
+  <si>
+    <t>Termo behavior</t>
+  </si>
+  <si>
+    <t>analysis feature</t>
+  </si>
+  <si>
+    <t>sensors</t>
   </si>
 </sst>
 </file>
@@ -1706,7 +1747,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1728,7 +1769,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>383</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1777,7 +1818,7 @@
     </row>
     <row r="6" spans="1:4" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>388</v>
+        <v>347</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>12</v>
@@ -1891,11 +1932,631 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4601F4ED-5DCC-4AED-9535-E950FE11A448}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="A1:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="37.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="82.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="37.6640625" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C560AA12-DAC7-40A4-AFE3-BA13199B1D7F}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="51.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" customWidth="1"/>
+    <col min="10" max="10" width="22.77734375" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" customWidth="1"/>
+    <col min="12" max="12" width="22.77734375" customWidth="1"/>
+    <col min="13" max="13" width="42.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="25" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="25" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F33FDE-D5A2-491B-A79C-E9AC783D9ADC}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1926,13 +2587,13 @@
         <v>34</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>355</v>
+        <v>314</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>35</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>356</v>
+        <v>315</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>36</v>
@@ -1941,13 +2602,13 @@
         <v>37</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>357</v>
+        <v>316</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>38</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>358</v>
+        <v>317</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>39</v>
@@ -1955,7 +2616,7 @@
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>40</v>
+        <v>359</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>24</v>
@@ -1967,13 +2628,13 @@
         <v>41</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>255</v>
+        <v>215</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>42</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>364</v>
+        <v>323</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -1986,7 +2647,7 @@
     </row>
     <row r="3" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>44</v>
+        <v>357</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>14</v>
@@ -1998,13 +2659,13 @@
         <v>45</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>359</v>
+        <v>318</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>372</v>
+        <v>331</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -2012,12 +2673,12 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10" t="s">
-        <v>389</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>46</v>
+        <v>360</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>16</v>
@@ -2029,13 +2690,13 @@
         <v>47</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>360</v>
+        <v>319</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>41</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -2048,7 +2709,7 @@
     </row>
     <row r="5" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>49</v>
+        <v>360</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>16</v>
@@ -2060,13 +2721,13 @@
         <v>50</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>361</v>
+        <v>320</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>41</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>373</v>
+        <v>332</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
@@ -2079,7 +2740,7 @@
     </row>
     <row r="6" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>51</v>
+        <v>358</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>26</v>
@@ -2091,13 +2752,13 @@
         <v>52</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>365</v>
+        <v>324</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>276</v>
+        <v>235</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -2110,7 +2771,7 @@
     </row>
     <row r="7" spans="1:13" s="25" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
-        <v>53</v>
+        <v>361</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>9</v>
@@ -2122,13 +2783,13 @@
         <v>41</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>319</v>
+        <v>278</v>
       </c>
       <c r="F7" s="25" t="s">
         <v>41</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="H7" s="23" t="s">
         <v>11</v>
@@ -2137,13 +2798,13 @@
         <v>54</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>368</v>
+        <v>327</v>
       </c>
       <c r="K7" s="22" t="s">
         <v>55</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>369</v>
+        <v>328</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>53</v>
@@ -2151,7 +2812,7 @@
     </row>
     <row r="8" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>56</v>
+        <v>361</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>9</v>
@@ -2163,13 +2824,13 @@
         <v>57</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>362</v>
+        <v>321</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>41</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>335</v>
+        <v>294</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -2182,7 +2843,7 @@
     </row>
     <row r="9" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>58</v>
+        <v>351</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>4</v>
@@ -2194,13 +2855,13 @@
         <v>41</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>370</v>
+        <v>329</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>59</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>366</v>
+        <v>325</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -2213,7 +2874,7 @@
     </row>
     <row r="10" spans="1:13" s="25" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>20</v>
@@ -2225,13 +2886,13 @@
         <v>41</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="F10" s="25" t="s">
         <v>41</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>318</v>
+        <v>277</v>
       </c>
       <c r="H10" s="22" t="s">
         <v>22</v>
@@ -2240,21 +2901,21 @@
         <v>61</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>385</v>
+        <v>344</v>
       </c>
       <c r="K10" s="22" t="s">
         <v>62</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>386</v>
+        <v>345</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>387</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>63</v>
+        <v>363</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>18</v>
@@ -2266,13 +2927,13 @@
         <v>64</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>363</v>
+        <v>322</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>41</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>275</v>
+        <v>234</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -2285,7 +2946,7 @@
     </row>
     <row r="12" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>66</v>
+        <v>364</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>30</v>
@@ -2297,13 +2958,13 @@
         <v>41</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>371</v>
+        <v>330</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>67</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>367</v>
+        <v>326</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -2314,20 +2975,381 @@
         <v>68</v>
       </c>
     </row>
+    <row r="13" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="25" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="K18" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="L18" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="25" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J21" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="L21" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="M21" s="22" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19F80CB-F092-4DED-9234-32DFC45B558F}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr applyStyles="1"/>
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2349,7 +3371,7 @@
         <v>70</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>354</v>
+        <v>313</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>71</v>
@@ -2362,9 +3384,9 @@
       </c>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>390</v>
+        <v>368</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -2379,12 +3401,12 @@
         <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -2399,12 +3421,12 @@
         <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>368</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -2419,12 +3441,12 @@
         <v>82</v>
       </c>
       <c r="F4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>266</v>
+        <v>369</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -2433,18 +3455,18 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>265</v>
+        <v>225</v>
       </c>
       <c r="E5" t="s">
         <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>367</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -2459,12 +3481,12 @@
         <v>82</v>
       </c>
       <c r="F6" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>370</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -2479,12 +3501,12 @@
         <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>371</v>
       </c>
       <c r="B8" t="s">
         <v>99</v>
@@ -2499,12 +3521,12 @@
         <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>372</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -2519,12 +3541,12 @@
         <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>373</v>
       </c>
       <c r="B10" t="s">
         <v>99</v>
@@ -2539,12 +3561,12 @@
         <v>75</v>
       </c>
       <c r="F10" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>374</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
@@ -2559,12 +3581,12 @@
         <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>375</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -2579,12 +3601,12 @@
         <v>75</v>
       </c>
       <c r="F12" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>376</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -2599,12 +3621,12 @@
         <v>82</v>
       </c>
       <c r="F13" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>197</v>
+        <v>377</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
@@ -2619,12 +3641,12 @@
         <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>378</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -2639,12 +3661,12 @@
         <v>82</v>
       </c>
       <c r="F15" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>199</v>
+        <v>379</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -2659,12 +3681,12 @@
         <v>82</v>
       </c>
       <c r="F16" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>200</v>
+        <v>380</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
@@ -2679,12 +3701,12 @@
         <v>82</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>201</v>
+        <v>381</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -2699,12 +3721,12 @@
         <v>82</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>202</v>
+        <v>382</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -2719,12 +3741,12 @@
         <v>82</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>203</v>
+        <v>383</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
@@ -2739,12 +3761,12 @@
         <v>82</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>204</v>
+        <v>384</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
@@ -2759,12 +3781,12 @@
         <v>82</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>205</v>
+        <v>385</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
@@ -2779,12 +3801,12 @@
         <v>82</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>206</v>
+        <v>386</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -2799,12 +3821,12 @@
         <v>75</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>386</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -2819,12 +3841,12 @@
         <v>75</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>206</v>
+        <v>386</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -2839,12 +3861,12 @@
         <v>75</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>207</v>
+        <v>387</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
@@ -2859,12 +3881,12 @@
         <v>75</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>208</v>
+        <v>388</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -2879,12 +3901,12 @@
         <v>82</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>209</v>
+        <v>389</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
@@ -2899,12 +3921,12 @@
         <v>75</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>210</v>
+        <v>390</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
@@ -2919,12 +3941,12 @@
         <v>75</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>211</v>
+        <v>391</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
@@ -2939,12 +3961,12 @@
         <v>82</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>216</v>
+        <v>392</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
@@ -2959,12 +3981,12 @@
         <v>82</v>
       </c>
       <c r="F31" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>217</v>
+        <v>393</v>
       </c>
       <c r="B32" t="s">
         <v>20</v>
@@ -2979,12 +4001,12 @@
         <v>82</v>
       </c>
       <c r="F32" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>224</v>
+        <v>394</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
@@ -2999,12 +4021,12 @@
         <v>133</v>
       </c>
       <c r="F33" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>225</v>
+        <v>395</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
@@ -3019,12 +4041,12 @@
         <v>142</v>
       </c>
       <c r="F34" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>226</v>
+        <v>396</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
@@ -3039,12 +4061,12 @@
         <v>142</v>
       </c>
       <c r="F35" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>228</v>
+        <v>397</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
@@ -3059,12 +4081,12 @@
         <v>76</v>
       </c>
       <c r="F36" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>229</v>
+        <v>398</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
@@ -3076,15 +4098,15 @@
         <v>140</v>
       </c>
       <c r="E37" t="s">
-        <v>334</v>
+        <v>293</v>
       </c>
       <c r="F37" t="s">
-        <v>333</v>
+        <v>292</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>232</v>
+        <v>399</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
@@ -3099,12 +4121,12 @@
         <v>76</v>
       </c>
       <c r="F38" t="s">
-        <v>338</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>233</v>
+        <v>400</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
@@ -3119,12 +4141,12 @@
         <v>77</v>
       </c>
       <c r="F39" t="s">
-        <v>339</v>
+        <v>298</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>234</v>
+        <v>401</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -3139,12 +4161,12 @@
         <v>77</v>
       </c>
       <c r="F40" t="s">
-        <v>340</v>
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>235</v>
+        <v>392</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
@@ -3159,12 +4181,12 @@
         <v>82</v>
       </c>
       <c r="F41" t="s">
-        <v>341</v>
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>236</v>
+        <v>402</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
@@ -3179,12 +4201,12 @@
         <v>76</v>
       </c>
       <c r="F42" t="s">
-        <v>342</v>
+        <v>301</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>237</v>
+        <v>403</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
@@ -3193,18 +4215,18 @@
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>393</v>
+        <v>350</v>
       </c>
       <c r="E43" t="s">
         <v>75</v>
       </c>
       <c r="F43" t="s">
-        <v>343</v>
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>238</v>
+        <v>404</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
@@ -3219,12 +4241,12 @@
         <v>76</v>
       </c>
       <c r="F44" t="s">
-        <v>344</v>
+        <v>303</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>240</v>
+        <v>405</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
@@ -3239,12 +4261,12 @@
         <v>76</v>
       </c>
       <c r="F45" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>249</v>
+        <v>406</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -3259,18 +4281,12 @@
         <v>82</v>
       </c>
       <c r="F46" t="s">
-        <v>352</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G46" xr:uid="{B19F80CB-F092-4DED-9234-32DFC45B558F}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="teq_tipo_equipo"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <dataValidations count="1">
+  <autoFilter ref="A1:G46" xr:uid="{B19F80CB-F092-4DED-9234-32DFC45B558F}"/>
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11" xr:uid="{C682601D-E683-4DA2-A853-C212B8D6B385}">
       <formula1>$L$2:$L$2</formula1>
     </dataValidation>
@@ -3279,11 +4295,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AFCDF92-DDD8-467D-BF61-440094865905}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -3306,7 +4322,7 @@
         <v>70</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>354</v>
+        <v>313</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>71</v>
@@ -3335,12 +4351,12 @@
         <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>372</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>392</v>
+        <v>349</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -3355,7 +4371,7 @@
         <v>73</v>
       </c>
       <c r="F3" t="s">
-        <v>251</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3375,7 +4391,7 @@
         <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>254</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3395,7 +4411,7 @@
         <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>255</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3415,12 +4431,12 @@
         <v>82</v>
       </c>
       <c r="F6" t="s">
-        <v>256</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -3435,12 +4451,12 @@
         <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>258</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -3455,12 +4471,12 @@
         <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>371</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -3475,12 +4491,12 @@
         <v>83</v>
       </c>
       <c r="F9" t="s">
-        <v>259</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -3495,12 +4511,12 @@
         <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>260</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -3515,12 +4531,12 @@
         <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -3535,12 +4551,12 @@
         <v>82</v>
       </c>
       <c r="F12" t="s">
-        <v>262</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -3555,12 +4571,12 @@
         <v>82</v>
       </c>
       <c r="F13" t="s">
-        <v>263</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -3575,12 +4591,12 @@
         <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>264</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s">
         <v>87</v>
@@ -3595,12 +4611,12 @@
         <v>75</v>
       </c>
       <c r="F15" t="s">
-        <v>270</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B16" t="s">
         <v>87</v>
@@ -3615,12 +4631,12 @@
         <v>82</v>
       </c>
       <c r="F16" t="s">
-        <v>272</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
         <v>87</v>
@@ -3635,12 +4651,12 @@
         <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>273</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
         <v>87</v>
@@ -3655,12 +4671,12 @@
         <v>90</v>
       </c>
       <c r="F18" t="s">
-        <v>274</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B19" t="s">
         <v>91</v>
@@ -3675,12 +4691,12 @@
         <v>75</v>
       </c>
       <c r="F19" t="s">
-        <v>271</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
         <v>91</v>
@@ -3695,12 +4711,12 @@
         <v>75</v>
       </c>
       <c r="F20" t="s">
-        <v>277</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
         <v>91</v>
@@ -3715,12 +4731,12 @@
         <v>75</v>
       </c>
       <c r="F21" t="s">
-        <v>278</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B22" t="s">
         <v>91</v>
@@ -3735,12 +4751,12 @@
         <v>74</v>
       </c>
       <c r="F22" t="s">
-        <v>279</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B23" t="s">
         <v>91</v>
@@ -3755,12 +4771,12 @@
         <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>280</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>282</v>
+        <v>241</v>
       </c>
       <c r="B24" t="s">
         <v>91</v>
@@ -3775,12 +4791,12 @@
         <v>74</v>
       </c>
       <c r="F24" t="s">
-        <v>281</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B25" t="s">
         <v>91</v>
@@ -3795,12 +4811,12 @@
         <v>75</v>
       </c>
       <c r="F25" t="s">
-        <v>283</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
@@ -3815,12 +4831,12 @@
         <v>75</v>
       </c>
       <c r="F26" t="s">
-        <v>275</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -3835,12 +4851,12 @@
         <v>74</v>
       </c>
       <c r="F27" t="s">
-        <v>376</v>
+        <v>335</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
@@ -3855,12 +4871,12 @@
         <v>77</v>
       </c>
       <c r="F28" t="s">
-        <v>377</v>
+        <v>336</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
@@ -3875,12 +4891,12 @@
         <v>75</v>
       </c>
       <c r="F29" t="s">
-        <v>276</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
@@ -3895,12 +4911,12 @@
         <v>82</v>
       </c>
       <c r="F30" t="s">
-        <v>284</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
@@ -3915,12 +4931,12 @@
         <v>77</v>
       </c>
       <c r="F31" t="s">
-        <v>285</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B32" t="s">
         <v>99</v>
@@ -3935,12 +4951,12 @@
         <v>75</v>
       </c>
       <c r="F32" t="s">
-        <v>286</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B33" t="s">
         <v>99</v>
@@ -3955,12 +4971,12 @@
         <v>73</v>
       </c>
       <c r="F33" t="s">
-        <v>287</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B34" t="s">
         <v>99</v>
@@ -3975,12 +4991,12 @@
         <v>75</v>
       </c>
       <c r="F34" t="s">
-        <v>291</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B35" t="s">
         <v>99</v>
@@ -3995,12 +5011,12 @@
         <v>75</v>
       </c>
       <c r="F35" t="s">
-        <v>292</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
         <v>26</v>
@@ -4015,12 +5031,12 @@
         <v>75</v>
       </c>
       <c r="F36" t="s">
-        <v>373</v>
+        <v>332</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>294</v>
+        <v>253</v>
       </c>
       <c r="B37" t="s">
         <v>26</v>
@@ -4035,12 +5051,12 @@
         <v>82</v>
       </c>
       <c r="F37" t="s">
-        <v>374</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B38" t="s">
         <v>26</v>
@@ -4055,12 +5071,12 @@
         <v>75</v>
       </c>
       <c r="F38" t="s">
-        <v>297</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>250</v>
+        <v>210</v>
       </c>
       <c r="B39" t="s">
         <v>26</v>
@@ -4075,12 +5091,12 @@
         <v>82</v>
       </c>
       <c r="F39" t="s">
-        <v>295</v>
+        <v>254</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B40" t="s">
         <v>26</v>
@@ -4095,12 +5111,12 @@
         <v>82</v>
       </c>
       <c r="F40" t="s">
-        <v>375</v>
+        <v>334</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
@@ -4115,12 +5131,12 @@
         <v>82</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>316</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
@@ -4135,12 +5151,12 @@
         <v>82</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>317</v>
+        <v>276</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="B43" t="s">
         <v>20</v>
@@ -4155,12 +5171,12 @@
         <v>75</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>318</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
@@ -4175,12 +5191,12 @@
         <v>82</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>320</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="B45" t="s">
         <v>20</v>
@@ -4195,12 +5211,12 @@
         <v>82</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>323</v>
+        <v>282</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="B46" t="s">
         <v>22</v>
@@ -4215,12 +5231,12 @@
         <v>133</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>324</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="B47" t="s">
         <v>22</v>
@@ -4235,12 +5251,12 @@
         <v>134</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>325</v>
+        <v>284</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="B48" t="s">
         <v>22</v>
@@ -4255,12 +5271,12 @@
         <v>82</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>326</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>222</v>
+        <v>196</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -4275,12 +5291,12 @@
         <v>75</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>319</v>
+        <v>278</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="B50" t="s">
         <v>9</v>
@@ -4295,12 +5311,12 @@
         <v>141</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>327</v>
+        <v>286</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
@@ -4315,12 +5331,12 @@
         <v>77</v>
       </c>
       <c r="F51" t="s">
-        <v>331</v>
+        <v>290</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -4335,12 +5351,12 @@
         <v>75</v>
       </c>
       <c r="F52" t="s">
-        <v>335</v>
+        <v>294</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="B53" t="s">
         <v>7</v>
@@ -4355,12 +5371,12 @@
         <v>83</v>
       </c>
       <c r="F53" t="s">
-        <v>337</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>239</v>
+        <v>201</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -4375,12 +5391,12 @@
         <v>77</v>
       </c>
       <c r="F54" t="s">
-        <v>345</v>
+        <v>304</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>241</v>
+        <v>202</v>
       </c>
       <c r="B55" t="s">
         <v>150</v>
@@ -4395,12 +5411,12 @@
         <v>75</v>
       </c>
       <c r="F55" t="s">
-        <v>336</v>
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>242</v>
+        <v>203</v>
       </c>
       <c r="B56" t="s">
         <v>150</v>
@@ -4415,12 +5431,12 @@
         <v>83</v>
       </c>
       <c r="F56" t="s">
-        <v>347</v>
+        <v>306</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="B57" t="s">
         <v>150</v>
@@ -4435,12 +5451,12 @@
         <v>77</v>
       </c>
       <c r="F57" t="s">
-        <v>348</v>
+        <v>307</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>244</v>
+        <v>205</v>
       </c>
       <c r="B58" t="s">
         <v>4</v>
@@ -4455,12 +5471,12 @@
         <v>75</v>
       </c>
       <c r="F58" t="s">
-        <v>370</v>
+        <v>329</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>245</v>
+        <v>206</v>
       </c>
       <c r="B59" t="s">
         <v>4</v>
@@ -4475,12 +5491,12 @@
         <v>83</v>
       </c>
       <c r="F59" t="s">
-        <v>349</v>
+        <v>308</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>246</v>
+        <v>207</v>
       </c>
       <c r="B60" t="s">
         <v>4</v>
@@ -4495,12 +5511,12 @@
         <v>77</v>
       </c>
       <c r="F60" t="s">
-        <v>350</v>
+        <v>309</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>247</v>
+        <v>208</v>
       </c>
       <c r="B61" t="s">
         <v>11</v>
@@ -4515,12 +5531,12 @@
         <v>73</v>
       </c>
       <c r="F61" t="s">
-        <v>351</v>
+        <v>310</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>248</v>
+        <v>209</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -4535,7 +5551,7 @@
         <v>77</v>
       </c>
       <c r="F62" t="s">
-        <v>353</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -4544,12 +5560,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8380192A-598A-46F3-A3CF-828328F6162A}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4562,19 +5578,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>378</v>
+        <v>337</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>379</v>
+        <v>338</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>381</v>
+        <v>340</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>382</v>
+        <v>341</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>380</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
switched flavored-request with flavored-keywords
</commit_message>
<xml_diff>
--- a/src/utils/data/semantics_data.xlsx
+++ b/src/utils/data/semantics_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauth\OneDrive\Desktop\sql_assistant_v3\src\utils\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9298A46-BA3E-4222-A9FA-74A435ABD281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C82C8A9-0880-4557-90EF-5FD09EBADBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="7992" windowWidth="23256" windowHeight="12456" tabRatio="757" activeTab="1" xr2:uid="{AFE3706E-D2E0-4CCB-B251-2FC4B29F0B89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="757" activeTab="4" xr2:uid="{AFE3706E-D2E0-4CCB-B251-2FC4B29F0B89}"/>
   </bookViews>
   <sheets>
     <sheet name="semantics_tables" sheetId="1" r:id="rId1"/>
@@ -1155,9 +1155,6 @@
     <t>abbreviature</t>
   </si>
   <si>
-    <t>sub fluid</t>
-  </si>
-  <si>
     <t>usage</t>
   </si>
   <si>
@@ -1267,6 +1264,9 @@
   </si>
   <si>
     <t>sensors</t>
+  </si>
+  <si>
+    <t>measurement system sub fluid</t>
   </si>
 </sst>
 </file>
@@ -1938,8 +1938,8 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="A1:C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3343,13 +3343,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19F80CB-F092-4DED-9234-32DFC45B558F}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr applyStyles="1"/>
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3384,7 +3384,7 @@
       </c>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>368</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>367</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>368</v>
       </c>
@@ -3446,7 +3446,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>369</v>
+        <v>406</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -3504,9 +3504,9 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B8" t="s">
         <v>99</v>
@@ -3524,9 +3524,9 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -3544,9 +3544,9 @@
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B10" t="s">
         <v>99</v>
@@ -3564,9 +3564,9 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
@@ -3584,9 +3584,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -3604,9 +3604,9 @@
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -3624,9 +3624,9 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
@@ -3644,9 +3644,9 @@
         <v>258</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -3664,9 +3664,9 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -3684,9 +3684,9 @@
         <v>260</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
@@ -3704,9 +3704,9 @@
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -3724,9 +3724,9 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -3744,9 +3744,9 @@
         <v>263</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
@@ -3764,9 +3764,9 @@
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
@@ -3784,9 +3784,9 @@
         <v>265</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
@@ -3804,9 +3804,9 @@
         <v>266</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -3824,9 +3824,9 @@
         <v>267</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -3844,9 +3844,9 @@
         <v>268</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -3864,9 +3864,9 @@
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
@@ -3884,9 +3884,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -3904,9 +3904,9 @@
         <v>271</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
@@ -3924,9 +3924,9 @@
         <v>272</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
@@ -3944,9 +3944,9 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
@@ -3964,9 +3964,9 @@
         <v>274</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
@@ -3984,9 +3984,9 @@
         <v>280</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B32" t="s">
         <v>20</v>
@@ -4004,9 +4004,9 @@
         <v>281</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
@@ -4024,9 +4024,9 @@
         <v>287</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
@@ -4044,9 +4044,9 @@
         <v>288</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
@@ -4064,9 +4064,9 @@
         <v>289</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
@@ -4084,9 +4084,9 @@
         <v>291</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
@@ -4104,9 +4104,9 @@
         <v>292</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
@@ -4124,9 +4124,9 @@
         <v>297</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
@@ -4144,9 +4144,9 @@
         <v>298</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -4164,9 +4164,9 @@
         <v>299</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
@@ -4184,9 +4184,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
@@ -4204,9 +4204,9 @@
         <v>301</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
@@ -4224,9 +4224,9 @@
         <v>302</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
@@ -4244,9 +4244,9 @@
         <v>303</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
@@ -4264,9 +4264,9 @@
         <v>305</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -4285,7 +4285,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G46" xr:uid="{B19F80CB-F092-4DED-9234-32DFC45B558F}"/>
+  <autoFilter ref="A1:G46" xr:uid="{B19F80CB-F092-4DED-9234-32DFC45B558F}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="med_sistema_medicion"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11" xr:uid="{C682601D-E683-4DA2-A853-C212B8D6B385}">
       <formula1>$L$2:$L$2</formula1>

</xml_diff>